<commit_message>
Strategy engine roots done trade type introduced
</commit_message>
<xml_diff>
--- a/Spreadsheats/Dropdowns.xlsx
+++ b/Spreadsheats/Dropdowns.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Stock</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Operator</t>
   </si>
   <si>
+    <t xml:space="preserve">Tradetype</t>
+  </si>
+  <si>
     <t xml:space="preserve">OIL</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t xml:space="preserve">&lt;</t>
   </si>
   <si>
+    <t xml:space="preserve">Long</t>
+  </si>
+  <si>
     <t xml:space="preserve">GAIL</t>
   </si>
   <si>
@@ -65,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short</t>
   </si>
   <si>
     <t xml:space="preserve">ADX</t>
@@ -177,13 +186,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -195,63 +204,72 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>16</v>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="0" t="s">
-        <v>17</v>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="0" t="s">
-        <v>18</v>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>